<commit_message>
Adding more features and support auto type
</commit_message>
<xml_diff>
--- a/inst/record/Performance record.xlsx
+++ b/inst/record/Performance record.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t xml:space="preserve">
 matMul&lt;-function(id,A,B){
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>opt1</t>
+  </si>
+  <si>
+    <t>opt2</t>
   </si>
 </sst>
 </file>
@@ -878,7 +881,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -995,6 +998,12 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
+      <c r="M6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
@@ -1006,6 +1015,15 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
+      <c r="L7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>2.8</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>

</xml_diff>

<commit_message>
1.Fix bugs in the matrix subsetting 2.Optimize the getOption function to make it easy to manage
</commit_message>
<xml_diff>
--- a/inst/record/Performance record.xlsx
+++ b/inst/record/Performance record.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t xml:space="preserve">
 matMul&lt;-function(id,A,B){
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>gpu:940m</t>
+  </si>
+  <si>
+    <t>opt1</t>
+  </si>
+  <si>
+    <t>opt2</t>
+  </si>
+  <si>
+    <t>version1</t>
+  </si>
+  <si>
+    <t>version2</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -125,13 +137,16 @@
   tmp=subRef(B,,ind)
   C=A%*%tmp
   return(C)
-}</t>
-  </si>
-  <si>
-    <t>opt1</t>
-  </si>
-  <si>
-    <t>opt2</t>
+}
+opt2
+tmp=subRef(A,ind,)
+  #tmp=A[ind,]
+  C=tmp%*%B
+  return(C)
+</t>
+  </si>
+  <si>
+    <t>no subRef</t>
   </si>
 </sst>
 </file>
@@ -881,7 +896,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -891,7 +906,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -941,8 +956,8 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="L3" t="s">
-        <v>13</v>
+      <c r="K3" t="s">
+        <v>12</v>
       </c>
       <c r="M3" t="s">
         <v>10</v>
@@ -1015,6 +1030,9 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
       <c r="L7" t="s">
         <v>14</v>
       </c>
@@ -1035,6 +1053,15 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
+      <c r="L8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>2.4</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
@@ -1046,6 +1073,15 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>3.1</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
@@ -1278,7 +1314,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="318.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>

</xml_diff>

<commit_message>
Support seq and : function
</commit_message>
<xml_diff>
--- a/inst/record/Performance record.xlsx
+++ b/inst/record/Performance record.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff\OneDrive\course material\work\Roswell park\gpuMagic\inst\record\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangj\OneDrive\course material\work\Roswell park\gpuMagic\inst\record\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t xml:space="preserve">
 matMul&lt;-function(id,A,B){
@@ -193,6 +193,21 @@
   </si>
   <si>
     <t>1600x</t>
+  </si>
+  <si>
+    <t>Nvidia</t>
+  </si>
+  <si>
+    <t>Intel</t>
+  </si>
+  <si>
+    <t>previous</t>
+  </si>
+  <si>
+    <t>now</t>
+  </si>
+  <si>
+    <t>Optimal</t>
   </si>
 </sst>
 </file>
@@ -536,12 +551,12 @@
       <selection sqref="A1:I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="13" max="13" width="13.6328125" customWidth="1"/>
+    <col min="13" max="13" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -560,7 +575,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -577,7 +592,7 @@
         <v>28.79</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -588,7 +603,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -599,7 +614,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -610,7 +625,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -621,7 +636,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -632,7 +647,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -643,7 +658,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -654,7 +669,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -665,7 +680,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -676,7 +691,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -687,7 +702,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -698,7 +713,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -709,7 +724,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -720,7 +735,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -731,7 +746,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -742,7 +757,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -753,7 +768,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -764,7 +779,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -775,7 +790,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -786,7 +801,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -797,7 +812,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -808,7 +823,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -819,7 +834,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -830,7 +845,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -841,7 +856,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -852,7 +867,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -863,7 +878,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -874,7 +889,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -885,7 +900,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -896,34 +911,34 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -942,16 +957,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="13" max="13" width="13.6328125" customWidth="1"/>
+    <col min="13" max="13" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -973,7 +988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -993,7 +1008,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1013,7 +1028,7 @@
         <v>6.59</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1033,7 +1048,7 @@
         <v>13.33</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1050,7 +1065,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1067,7 +1082,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1090,7 +1105,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1110,7 +1125,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1130,7 +1145,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1141,7 +1156,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1152,7 +1167,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1163,7 +1178,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1174,7 +1189,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1185,7 +1200,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1196,7 +1211,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1207,7 +1222,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1218,7 +1233,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1229,7 +1244,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1240,7 +1255,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1251,7 +1266,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1262,7 +1277,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1273,7 +1288,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1284,7 +1299,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1295,7 +1310,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1306,7 +1321,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1317,7 +1332,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1328,7 +1343,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1339,7 +1354,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1350,7 +1365,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1361,7 +1376,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:9" ht="318.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="318.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1372,34 +1387,34 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1422,9 +1437,9 @@
       <selection activeCell="B1" sqref="B1:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1439,7 +1454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1449,7 +1464,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1459,56 +1474,56 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -1526,18 +1541,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="1" max="1" width="19.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1584,7 +1599,7 @@
         <v>43451</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1637,7 +1652,7 @@
         <v>5.0599999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1690,7 +1705,7 @@
         <v>5.62</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1740,7 +1755,7 @@
         <v>4.08</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1790,7 +1805,7 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1798,7 +1813,7 @@
         <v>6.59</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>1070</v>
       </c>
@@ -1848,9 +1863,65 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="L8" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>9.92</v>
+      </c>
+      <c r="D14">
+        <v>1.71</v>
+      </c>
+      <c r="E14">
+        <v>4.55</v>
+      </c>
+      <c r="F14">
+        <v>3.2949999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15">
+        <v>2.8</v>
+      </c>
+      <c r="D15">
+        <v>1.85</v>
+      </c>
+      <c r="E15">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>3.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>